<commit_message>
NO-ISSUE Fix excel template
</commit_message>
<xml_diff>
--- a/container-packing_template.xlsx
+++ b/container-packing_template.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27827"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="20" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA71B1E9-0313-4C96-B850-37046AAF7C6F}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="8">
   <si>
     <t>케이블 번호
 (화물)</t>
@@ -54,18 +54,27 @@
   <si>
     <t> </t>
   </si>
+  <si>
+    <t>Do not remove this comment</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -96,7 +105,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <fgColor theme="2" tint="-0.0999500006437302"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -110,32 +119,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
@@ -146,7 +129,6 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left/>
@@ -159,7 +141,30 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
     <border>
       <left style="thin">
@@ -170,7 +175,6 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -183,7 +187,6 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left/>
@@ -194,34 +197,139 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="15" builtinId="5"/>
+    <cellStyle name="Currency" xfId="16" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="17" builtinId="7"/>
+    <cellStyle name="Comma" xfId="18" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="19" builtinId="6"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -529,23 +637,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="5" width="9.140625" style="2"/>
-    <col min="6" max="6" width="9.140625" style="6"/>
-    <col min="7" max="7" width="9.140625" style="4"/>
+    <col min="2" max="5" width="9.14285714285714" style="2"/>
+    <col min="6" max="6" width="9.14285714285714" style="6"/>
+    <col min="7" max="7" width="9.14285714285714" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" ht="15">
       <c r="A1" s="8"/>
-      <c r="B1" s="7"/>
+      <c r="B1" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
@@ -553,7 +663,7 @@
       <c r="G1" s="7"/>
       <c r="H1" s="8"/>
     </row>
-    <row r="2" spans="1:8" ht="41.25">
+    <row r="2" spans="2:7" ht="41.25">
       <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
@@ -573,7 +683,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="2:7" ht="15">
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
@@ -593,7 +703,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="2:7" ht="15">
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
@@ -613,7 +723,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="2:7" ht="15">
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
@@ -633,7 +743,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="2:7" ht="15">
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -653,7 +763,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="2:7" ht="15">
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
@@ -673,7 +783,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="2:7" ht="15">
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
@@ -693,7 +803,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="2:7" ht="15">
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
@@ -713,7 +823,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="2:7" ht="15">
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
@@ -733,7 +843,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="2:7" ht="15">
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
@@ -753,7 +863,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="2:7" ht="15">
       <c r="B12" s="1" t="s">
         <v>6</v>
       </c>
@@ -773,7 +883,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="2:7" ht="15">
       <c r="B13" s="1" t="s">
         <v>6</v>
       </c>
@@ -793,7 +903,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="2:7" ht="15">
       <c r="B14" s="1" t="s">
         <v>6</v>
       </c>
@@ -813,7 +923,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="2:7" ht="15">
       <c r="B15" s="1" t="s">
         <v>6</v>
       </c>
@@ -833,7 +943,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="2:7" ht="15">
       <c r="B16" s="1" t="s">
         <v>6</v>
       </c>
@@ -853,7 +963,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="2:7">
+    <row r="17" spans="2:7" ht="15">
       <c r="B17" s="1" t="s">
         <v>6</v>
       </c>
@@ -873,7 +983,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="2:7">
+    <row r="18" spans="2:7" ht="15">
       <c r="B18" s="1" t="s">
         <v>6</v>
       </c>
@@ -893,7 +1003,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="2:7">
+    <row r="19" spans="2:7" ht="15">
       <c r="B19" s="1" t="s">
         <v>6</v>
       </c>
@@ -913,7 +1023,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="2:7">
+    <row r="20" spans="2:7" ht="15">
       <c r="B20" s="1" t="s">
         <v>6</v>
       </c>
@@ -933,7 +1043,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="2:7">
+    <row r="21" spans="2:7" ht="15">
       <c r="B21" s="1" t="s">
         <v>6</v>
       </c>
@@ -953,7 +1063,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="2:7">
+    <row r="22" spans="2:7" ht="15">
       <c r="B22" s="1" t="s">
         <v>6</v>
       </c>
@@ -973,7 +1083,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="2:7">
+    <row r="23" spans="2:7" ht="15">
       <c r="B23" s="1" t="s">
         <v>6</v>
       </c>
@@ -993,7 +1103,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="2:7">
+    <row r="24" spans="2:7" ht="15">
       <c r="B24" s="1" t="s">
         <v>6</v>
       </c>
@@ -1013,7 +1123,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="2:7">
+    <row r="25" spans="2:7" ht="15">
       <c r="B25" s="1" t="s">
         <v>6</v>
       </c>
@@ -1033,7 +1143,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="2:7">
+    <row r="26" spans="2:7" ht="15">
       <c r="B26" s="1" t="s">
         <v>6</v>
       </c>
@@ -1053,7 +1163,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="2:7">
+    <row r="27" spans="2:7" ht="15">
       <c r="B27" s="1" t="s">
         <v>6</v>
       </c>
@@ -1073,7 +1183,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="2:7">
+    <row r="28" spans="2:7" ht="15">
       <c r="B28" s="1" t="s">
         <v>6</v>
       </c>
@@ -1093,7 +1203,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="2:7">
+    <row r="29" spans="2:7" ht="15">
       <c r="B29" s="1" t="s">
         <v>6</v>
       </c>
@@ -1113,7 +1223,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="2:7">
+    <row r="30" spans="2:7" ht="15">
       <c r="B30" s="1" t="s">
         <v>6</v>
       </c>
@@ -1133,7 +1243,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="2:7">
+    <row r="31" spans="2:7" ht="15">
       <c r="B31" s="1" t="s">
         <v>6</v>
       </c>
@@ -1153,7 +1263,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="2:7">
+    <row r="32" spans="2:7" ht="15">
       <c r="B32" s="1" t="s">
         <v>6</v>
       </c>
@@ -1173,7 +1283,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="2:7">
+    <row r="33" spans="2:7" ht="15">
       <c r="B33" s="1" t="s">
         <v>6</v>
       </c>
@@ -1193,7 +1303,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="2:7">
+    <row r="34" spans="2:7" ht="15">
       <c r="B34" s="1" t="s">
         <v>6</v>
       </c>
@@ -1213,7 +1323,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="2:7">
+    <row r="35" spans="2:7" ht="15">
       <c r="B35" s="1" t="s">
         <v>6</v>
       </c>
@@ -1233,7 +1343,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="2:7">
+    <row r="36" spans="2:7" ht="15">
       <c r="B36" s="1" t="s">
         <v>6</v>
       </c>
@@ -1253,7 +1363,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="2:7">
+    <row r="37" spans="2:7" ht="15">
       <c r="B37" s="1" t="s">
         <v>6</v>
       </c>
@@ -1273,7 +1383,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="2:7">
+    <row r="38" spans="2:7" ht="15">
       <c r="B38" s="1" t="s">
         <v>6</v>
       </c>
@@ -1293,7 +1403,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="2:7">
+    <row r="39" spans="2:7" ht="15">
       <c r="B39" s="1" t="s">
         <v>6</v>
       </c>
@@ -1313,7 +1423,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="2:7">
+    <row r="40" spans="2:7" ht="15">
       <c r="B40" s="1" t="s">
         <v>6</v>
       </c>
@@ -1333,7 +1443,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="2:7">
+    <row r="41" spans="2:7" ht="15">
       <c r="B41" s="1" t="s">
         <v>6</v>
       </c>
@@ -1353,7 +1463,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="2:7">
+    <row r="42" spans="2:7" ht="15">
       <c r="B42" s="1" t="s">
         <v>6</v>
       </c>
@@ -1373,7 +1483,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="2:7">
+    <row r="43" spans="2:7" ht="15">
       <c r="B43" s="1" t="s">
         <v>6</v>
       </c>
@@ -1393,7 +1503,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="2:7">
+    <row r="44" spans="2:7" ht="15">
       <c r="B44" s="1" t="s">
         <v>6</v>
       </c>
@@ -1413,7 +1523,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="2:7">
+    <row r="45" spans="2:7" ht="15">
       <c r="B45" s="1" t="s">
         <v>6</v>
       </c>

</xml_diff>